<commit_message>
finished draft of power rankings, with all arrows and colors complete now
</commit_message>
<xml_diff>
--- a/power_ranking.xlsx
+++ b/power_ranking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C217"/>
+  <dimension ref="A1:C265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3258,6 +3258,630 @@
         <v>12</v>
       </c>
     </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>19</v>
+      </c>
+      <c r="C218" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>19</v>
+      </c>
+      <c r="C219" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Sith Happens</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>19</v>
+      </c>
+      <c r="C220" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Apex Predators</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>19</v>
+      </c>
+      <c r="C221" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>19</v>
+      </c>
+      <c r="C222" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>19</v>
+      </c>
+      <c r="C223" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Drafted by AI</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>19</v>
+      </c>
+      <c r="C224" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>19</v>
+      </c>
+      <c r="C225" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Bring the heat</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>19</v>
+      </c>
+      <c r="C226" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>19</v>
+      </c>
+      <c r="C227" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>19</v>
+      </c>
+      <c r="C228" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>19</v>
+      </c>
+      <c r="C229" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>20</v>
+      </c>
+      <c r="C230" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>20</v>
+      </c>
+      <c r="C231" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Sith Happens</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>20</v>
+      </c>
+      <c r="C232" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Apex Predators</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>20</v>
+      </c>
+      <c r="C233" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>20</v>
+      </c>
+      <c r="C234" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>20</v>
+      </c>
+      <c r="C235" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Drafted by AI</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>20</v>
+      </c>
+      <c r="C236" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>20</v>
+      </c>
+      <c r="C237" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Bring the heat</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>20</v>
+      </c>
+      <c r="C238" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>20</v>
+      </c>
+      <c r="C239" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>20</v>
+      </c>
+      <c r="C240" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>20</v>
+      </c>
+      <c r="C241" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>21</v>
+      </c>
+      <c r="C242" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>21</v>
+      </c>
+      <c r="C243" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Sith Happens</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>21</v>
+      </c>
+      <c r="C244" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Apex Predators</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>21</v>
+      </c>
+      <c r="C245" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>21</v>
+      </c>
+      <c r="C246" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>21</v>
+      </c>
+      <c r="C247" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Drafted by AI</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>21</v>
+      </c>
+      <c r="C248" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>21</v>
+      </c>
+      <c r="C249" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Bring the heat</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>21</v>
+      </c>
+      <c r="C250" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>21</v>
+      </c>
+      <c r="C251" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>21</v>
+      </c>
+      <c r="C252" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>21</v>
+      </c>
+      <c r="C253" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Baby Back Gibbs</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>22</v>
+      </c>
+      <c r="C254" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Magic Mikaela</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>22</v>
+      </c>
+      <c r="C255" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Sith Happens</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>22</v>
+      </c>
+      <c r="C256" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Apex Predators</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>22</v>
+      </c>
+      <c r="C257" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Mighty Rubber Ducks</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>22</v>
+      </c>
+      <c r="C258" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Compile and Conquer</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>22</v>
+      </c>
+      <c r="C259" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Drafted by AI</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>22</v>
+      </c>
+      <c r="C260" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Aida's Astounding Team</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>22</v>
+      </c>
+      <c r="C261" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Bring the heat</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>22</v>
+      </c>
+      <c r="C262" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Kelly's Deluxe Team</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>22</v>
+      </c>
+      <c r="C263" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Boomer Sooners</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>22</v>
+      </c>
+      <c r="C264" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Kuppenheimer</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>22</v>
+      </c>
+      <c r="C265" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated power ranking df with correct weeks
</commit_message>
<xml_diff>
--- a/power_ranking.xlsx
+++ b/power_ranking.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C265"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3102,786 +3102,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>Baby Back Gibbs</t>
-        </is>
-      </c>
-      <c r="B206" t="n">
-        <v>18</v>
-      </c>
-      <c r="C206" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>Magic Mikaela</t>
-        </is>
-      </c>
-      <c r="B207" t="n">
-        <v>18</v>
-      </c>
-      <c r="C207" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>Sith Happens</t>
-        </is>
-      </c>
-      <c r="B208" t="n">
-        <v>18</v>
-      </c>
-      <c r="C208" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>Apex Predators</t>
-        </is>
-      </c>
-      <c r="B209" t="n">
-        <v>18</v>
-      </c>
-      <c r="C209" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>Mighty Rubber Ducks</t>
-        </is>
-      </c>
-      <c r="B210" t="n">
-        <v>18</v>
-      </c>
-      <c r="C210" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>Compile and Conquer</t>
-        </is>
-      </c>
-      <c r="B211" t="n">
-        <v>18</v>
-      </c>
-      <c r="C211" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>Drafted by AI</t>
-        </is>
-      </c>
-      <c r="B212" t="n">
-        <v>18</v>
-      </c>
-      <c r="C212" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>Aida's Astounding Team</t>
-        </is>
-      </c>
-      <c r="B213" t="n">
-        <v>18</v>
-      </c>
-      <c r="C213" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
-        <is>
-          <t>Bring the heat</t>
-        </is>
-      </c>
-      <c r="B214" t="n">
-        <v>18</v>
-      </c>
-      <c r="C214" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t>Kelly's Deluxe Team</t>
-        </is>
-      </c>
-      <c r="B215" t="n">
-        <v>18</v>
-      </c>
-      <c r="C215" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t>Boomer Sooners</t>
-        </is>
-      </c>
-      <c r="B216" t="n">
-        <v>18</v>
-      </c>
-      <c r="C216" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>Kuppenheimer</t>
-        </is>
-      </c>
-      <c r="B217" t="n">
-        <v>18</v>
-      </c>
-      <c r="C217" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t>Baby Back Gibbs</t>
-        </is>
-      </c>
-      <c r="B218" t="n">
-        <v>19</v>
-      </c>
-      <c r="C218" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>Magic Mikaela</t>
-        </is>
-      </c>
-      <c r="B219" t="n">
-        <v>19</v>
-      </c>
-      <c r="C219" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="inlineStr">
-        <is>
-          <t>Sith Happens</t>
-        </is>
-      </c>
-      <c r="B220" t="n">
-        <v>19</v>
-      </c>
-      <c r="C220" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
-        <is>
-          <t>Apex Predators</t>
-        </is>
-      </c>
-      <c r="B221" t="n">
-        <v>19</v>
-      </c>
-      <c r="C221" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="inlineStr">
-        <is>
-          <t>Mighty Rubber Ducks</t>
-        </is>
-      </c>
-      <c r="B222" t="n">
-        <v>19</v>
-      </c>
-      <c r="C222" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>Compile and Conquer</t>
-        </is>
-      </c>
-      <c r="B223" t="n">
-        <v>19</v>
-      </c>
-      <c r="C223" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="inlineStr">
-        <is>
-          <t>Drafted by AI</t>
-        </is>
-      </c>
-      <c r="B224" t="n">
-        <v>19</v>
-      </c>
-      <c r="C224" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="inlineStr">
-        <is>
-          <t>Aida's Astounding Team</t>
-        </is>
-      </c>
-      <c r="B225" t="n">
-        <v>19</v>
-      </c>
-      <c r="C225" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>Bring the heat</t>
-        </is>
-      </c>
-      <c r="B226" t="n">
-        <v>19</v>
-      </c>
-      <c r="C226" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
-        <is>
-          <t>Kelly's Deluxe Team</t>
-        </is>
-      </c>
-      <c r="B227" t="n">
-        <v>19</v>
-      </c>
-      <c r="C227" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
-        <is>
-          <t>Boomer Sooners</t>
-        </is>
-      </c>
-      <c r="B228" t="n">
-        <v>19</v>
-      </c>
-      <c r="C228" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>Kuppenheimer</t>
-        </is>
-      </c>
-      <c r="B229" t="n">
-        <v>19</v>
-      </c>
-      <c r="C229" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>Baby Back Gibbs</t>
-        </is>
-      </c>
-      <c r="B230" t="n">
-        <v>20</v>
-      </c>
-      <c r="C230" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="inlineStr">
-        <is>
-          <t>Magic Mikaela</t>
-        </is>
-      </c>
-      <c r="B231" t="n">
-        <v>20</v>
-      </c>
-      <c r="C231" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="inlineStr">
-        <is>
-          <t>Sith Happens</t>
-        </is>
-      </c>
-      <c r="B232" t="n">
-        <v>20</v>
-      </c>
-      <c r="C232" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="inlineStr">
-        <is>
-          <t>Apex Predators</t>
-        </is>
-      </c>
-      <c r="B233" t="n">
-        <v>20</v>
-      </c>
-      <c r="C233" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="inlineStr">
-        <is>
-          <t>Mighty Rubber Ducks</t>
-        </is>
-      </c>
-      <c r="B234" t="n">
-        <v>20</v>
-      </c>
-      <c r="C234" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="inlineStr">
-        <is>
-          <t>Compile and Conquer</t>
-        </is>
-      </c>
-      <c r="B235" t="n">
-        <v>20</v>
-      </c>
-      <c r="C235" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="inlineStr">
-        <is>
-          <t>Drafted by AI</t>
-        </is>
-      </c>
-      <c r="B236" t="n">
-        <v>20</v>
-      </c>
-      <c r="C236" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="inlineStr">
-        <is>
-          <t>Aida's Astounding Team</t>
-        </is>
-      </c>
-      <c r="B237" t="n">
-        <v>20</v>
-      </c>
-      <c r="C237" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="inlineStr">
-        <is>
-          <t>Bring the heat</t>
-        </is>
-      </c>
-      <c r="B238" t="n">
-        <v>20</v>
-      </c>
-      <c r="C238" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="inlineStr">
-        <is>
-          <t>Kelly's Deluxe Team</t>
-        </is>
-      </c>
-      <c r="B239" t="n">
-        <v>20</v>
-      </c>
-      <c r="C239" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="inlineStr">
-        <is>
-          <t>Boomer Sooners</t>
-        </is>
-      </c>
-      <c r="B240" t="n">
-        <v>20</v>
-      </c>
-      <c r="C240" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="inlineStr">
-        <is>
-          <t>Kuppenheimer</t>
-        </is>
-      </c>
-      <c r="B241" t="n">
-        <v>20</v>
-      </c>
-      <c r="C241" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="inlineStr">
-        <is>
-          <t>Baby Back Gibbs</t>
-        </is>
-      </c>
-      <c r="B242" t="n">
-        <v>21</v>
-      </c>
-      <c r="C242" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="inlineStr">
-        <is>
-          <t>Magic Mikaela</t>
-        </is>
-      </c>
-      <c r="B243" t="n">
-        <v>21</v>
-      </c>
-      <c r="C243" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="inlineStr">
-        <is>
-          <t>Sith Happens</t>
-        </is>
-      </c>
-      <c r="B244" t="n">
-        <v>21</v>
-      </c>
-      <c r="C244" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="inlineStr">
-        <is>
-          <t>Apex Predators</t>
-        </is>
-      </c>
-      <c r="B245" t="n">
-        <v>21</v>
-      </c>
-      <c r="C245" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="inlineStr">
-        <is>
-          <t>Mighty Rubber Ducks</t>
-        </is>
-      </c>
-      <c r="B246" t="n">
-        <v>21</v>
-      </c>
-      <c r="C246" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="inlineStr">
-        <is>
-          <t>Compile and Conquer</t>
-        </is>
-      </c>
-      <c r="B247" t="n">
-        <v>21</v>
-      </c>
-      <c r="C247" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="inlineStr">
-        <is>
-          <t>Drafted by AI</t>
-        </is>
-      </c>
-      <c r="B248" t="n">
-        <v>21</v>
-      </c>
-      <c r="C248" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="inlineStr">
-        <is>
-          <t>Aida's Astounding Team</t>
-        </is>
-      </c>
-      <c r="B249" t="n">
-        <v>21</v>
-      </c>
-      <c r="C249" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="inlineStr">
-        <is>
-          <t>Bring the heat</t>
-        </is>
-      </c>
-      <c r="B250" t="n">
-        <v>21</v>
-      </c>
-      <c r="C250" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="inlineStr">
-        <is>
-          <t>Kelly's Deluxe Team</t>
-        </is>
-      </c>
-      <c r="B251" t="n">
-        <v>21</v>
-      </c>
-      <c r="C251" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="inlineStr">
-        <is>
-          <t>Boomer Sooners</t>
-        </is>
-      </c>
-      <c r="B252" t="n">
-        <v>21</v>
-      </c>
-      <c r="C252" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="inlineStr">
-        <is>
-          <t>Kuppenheimer</t>
-        </is>
-      </c>
-      <c r="B253" t="n">
-        <v>21</v>
-      </c>
-      <c r="C253" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="inlineStr">
-        <is>
-          <t>Baby Back Gibbs</t>
-        </is>
-      </c>
-      <c r="B254" t="n">
-        <v>22</v>
-      </c>
-      <c r="C254" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="inlineStr">
-        <is>
-          <t>Magic Mikaela</t>
-        </is>
-      </c>
-      <c r="B255" t="n">
-        <v>22</v>
-      </c>
-      <c r="C255" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="inlineStr">
-        <is>
-          <t>Sith Happens</t>
-        </is>
-      </c>
-      <c r="B256" t="n">
-        <v>22</v>
-      </c>
-      <c r="C256" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="inlineStr">
-        <is>
-          <t>Apex Predators</t>
-        </is>
-      </c>
-      <c r="B257" t="n">
-        <v>22</v>
-      </c>
-      <c r="C257" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="inlineStr">
-        <is>
-          <t>Mighty Rubber Ducks</t>
-        </is>
-      </c>
-      <c r="B258" t="n">
-        <v>22</v>
-      </c>
-      <c r="C258" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="inlineStr">
-        <is>
-          <t>Compile and Conquer</t>
-        </is>
-      </c>
-      <c r="B259" t="n">
-        <v>22</v>
-      </c>
-      <c r="C259" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="inlineStr">
-        <is>
-          <t>Drafted by AI</t>
-        </is>
-      </c>
-      <c r="B260" t="n">
-        <v>22</v>
-      </c>
-      <c r="C260" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="inlineStr">
-        <is>
-          <t>Aida's Astounding Team</t>
-        </is>
-      </c>
-      <c r="B261" t="n">
-        <v>22</v>
-      </c>
-      <c r="C261" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="inlineStr">
-        <is>
-          <t>Bring the heat</t>
-        </is>
-      </c>
-      <c r="B262" t="n">
-        <v>22</v>
-      </c>
-      <c r="C262" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="inlineStr">
-        <is>
-          <t>Kelly's Deluxe Team</t>
-        </is>
-      </c>
-      <c r="B263" t="n">
-        <v>22</v>
-      </c>
-      <c r="C263" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="inlineStr">
-        <is>
-          <t>Boomer Sooners</t>
-        </is>
-      </c>
-      <c r="B264" t="n">
-        <v>22</v>
-      </c>
-      <c r="C264" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="inlineStr">
-        <is>
-          <t>Kuppenheimer</t>
-        </is>
-      </c>
-      <c r="B265" t="n">
-        <v>22</v>
-      </c>
-      <c r="C265" t="n">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>